<commit_message>
:bento: update 2.1 160222
</commit_message>
<xml_diff>
--- a/附件/基金定投18——160222.xlsx
+++ b/附件/基金定投18——160222.xlsx
@@ -33,34 +33,34 @@
     <t>最新净值</t>
   </si>
   <si>
+    <t>平均净值</t>
+  </si>
+  <si>
+    <t>总额</t>
+  </si>
+  <si>
     <t>1.18（四）1.4079</t>
   </si>
   <si>
-    <t>平均净值</t>
+    <t>总份数</t>
   </si>
   <si>
     <t>1.11（四）</t>
   </si>
   <si>
-    <t>总额</t>
+    <t>当前收益</t>
   </si>
   <si>
     <t>12.27（三）</t>
   </si>
   <si>
-    <t>总份数</t>
+    <t>收益百分比</t>
   </si>
   <si>
     <t>12.22（五）</t>
   </si>
   <si>
-    <t>当前收益</t>
-  </si>
-  <si>
     <t>12.14(四)</t>
-  </si>
-  <si>
-    <t>收益百分比</t>
   </si>
   <si>
     <t>12.7(四)</t>
@@ -84,11 +84,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,7 +100,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,6 +172,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -195,13 +202,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,23 +226,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,18 +256,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -287,67 +310,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,30 +418,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -408,42 +437,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,52 +614,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -678,95 +671,95 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -776,19 +769,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1151,10 +1147,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1165,7 +1161,7 @@
     <col min="7" max="7" width="12.625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" ht="14.25" spans="1:1">
       <c r="A1">
         <v>160222</v>
       </c>
@@ -1187,151 +1183,152 @@
         <v>4</v>
       </c>
       <c r="G2" s="2">
-        <v>1.43</v>
+        <v>1.379</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="A3" s="3">
+        <v>43130</v>
+      </c>
+      <c r="B3">
+        <v>1.379</v>
+      </c>
+      <c r="C3">
+        <v>217.5</v>
+      </c>
+      <c r="D3">
+        <v>160.85</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>200</v>
-      </c>
-      <c r="D3">
-        <v>142.36</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="5">
+        <f>AVERAGE(B5:B1000003)</f>
+        <v>1.30362857142857</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3">
+        <v>43124</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1.4142</v>
+      </c>
+      <c r="C4">
+        <v>191.1</v>
+      </c>
+      <c r="D4">
+        <v>135.13</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4">
-        <f>AVERAGE(B3:B1000001)</f>
-        <v>1.30362857142857</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>1.406</v>
-      </c>
-      <c r="C4">
-        <v>200</v>
-      </c>
-      <c r="D4">
-        <v>142.25</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="4">
-        <f>SUM(C3:C1000001)</f>
+      <c r="G4" s="5">
+        <f>SUM(C5:C1000003)</f>
         <v>1606</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>1.3125</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B5" s="6"/>
       <c r="C5">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="D5">
-        <v>163.05</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="4">
-        <f>SUM(D3:D1000001)</f>
+        <v>142.36</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5">
+        <f>SUM(D5:D1000003)</f>
         <v>1225.17</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1.406</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="D6">
+        <v>142.25</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="5">
+        <f>(G5*G2-G4)</f>
+        <v>83.5094300000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>1.3484</v>
-      </c>
-      <c r="C6">
-        <v>180</v>
-      </c>
-      <c r="D6">
-        <v>133.49</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="B7" s="6">
+        <v>1.3125</v>
+      </c>
+      <c r="C7">
+        <v>214</v>
+      </c>
+      <c r="D7">
+        <v>163.05</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="4">
-        <f>(G5*G2-G4)</f>
-        <v>145.9931</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" spans="1:7">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>1.3103</v>
-      </c>
-      <c r="C7">
-        <v>190</v>
-      </c>
-      <c r="D7">
-        <v>145</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="G7" s="8">
         <f>(G6/G5)</f>
-        <v>0.119161504117796</v>
+        <v>0.068161504117796</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1.3484</v>
+      </c>
+      <c r="C8">
+        <v>180</v>
+      </c>
+      <c r="D8">
+        <v>133.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.3103</v>
+      </c>
+      <c r="C9">
+        <v>190</v>
+      </c>
+      <c r="D9">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
+      <c r="B10" s="6">
         <v>1.2147</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>208</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <v>171.24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="7">
-        <v>43434</v>
-      </c>
-      <c r="B9">
-        <v>1.2161</v>
-      </c>
-      <c r="C9">
-        <v>214</v>
-      </c>
-      <c r="D9">
-        <v>175.97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="7">
-        <v>43424</v>
-      </c>
-      <c r="B10">
-        <v>1.3174</v>
-      </c>
-      <c r="C10">
-        <v>200</v>
-      </c>
-      <c r="D10">
-        <v>151.81</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -1340,31 +1337,83 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="6:7">
+    <row r="11" spans="1:7">
+      <c r="A11" s="3">
+        <v>43434</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.2161</v>
+      </c>
+      <c r="C11">
+        <v>214</v>
+      </c>
+      <c r="D11">
+        <v>175.97</v>
+      </c>
       <c r="F11" t="s">
         <v>17</v>
       </c>
       <c r="G11">
-        <v>1.4142</v>
-      </c>
-    </row>
-    <row r="12" spans="6:7">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3">
+        <v>43424</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1.3174</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <v>151.81</v>
+      </c>
       <c r="F12" t="s">
         <v>18</v>
       </c>
       <c r="G12">
         <f>(G11/G3)*G10*(1-G7)</f>
-        <v>191.109926274712</v>
-      </c>
-    </row>
-    <row r="13" spans="6:7">
+        <v>192.996992703593</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="6"/>
       <c r="F13" t="s">
         <v>19</v>
       </c>
       <c r="G13">
-        <f>(G11/G3)*G10</f>
-        <v>216.96363995003</v>
-      </c>
+        <f>(G11/G3)*G10*1.05</f>
+        <v>217.469919126833</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G6">

</xml_diff>

<commit_message>
:bento: update 2 files
</commit_message>
<xml_diff>
--- a/附件/基金定投18——160222.xlsx
+++ b/附件/基金定投18——160222.xlsx
@@ -83,10 +83,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -99,6 +99,29 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,50 +181,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +206,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -256,6 +256,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -310,6 +340,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -359,48 +401,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,6 +512,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -527,15 +551,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -547,36 +562,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,6 +586,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -617,10 +617,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -629,133 +629,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1158,7 +1158,7 @@
     <col min="1" max="1" width="9.125"/>
     <col min="2" max="2" width="12.625"/>
     <col min="6" max="6" width="13.625" customWidth="1"/>
-    <col min="7" max="7" width="12.625"/>
+    <col min="7" max="7" width="13.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" spans="1:1">
@@ -1183,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="2">
-        <v>1.379</v>
+        <v>1.3059</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="G6" s="5">
         <f>(G5*G2-G4)</f>
-        <v>83.5094300000001</v>
+        <v>-6.05049699999972</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="G7" s="8">
         <f>(G6/G5)</f>
-        <v>0.068161504117796</v>
+        <v>-0.00493849588220388</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1354,7 +1354,7 @@
         <v>17</v>
       </c>
       <c r="G11">
-        <v>1.35</v>
+        <v>1.2751</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="G12">
         <f>(G11/G3)*G10*(1-G7)</f>
-        <v>192.996992703593</v>
+        <v>196.589289953225</v>
       </c>
     </row>
     <row r="13" spans="2:7">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="G13">
         <f>(G11/G3)*G10*1.05</f>
-        <v>217.469919126833</v>
+        <v>205.404365836018</v>
       </c>
     </row>
     <row r="14" spans="2:2">

</xml_diff>